<commit_message>
amc bug fix + chantier orange dev
</commit_message>
<xml_diff>
--- a/Lamia/DBASE/create/Base2_chantier_0_1.xlsx
+++ b/Lamia/DBASE/create/Base2_chantier_0_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrice.verchere\PycharmProjects\Lamia\Lamia\DBASE\create\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AAC906-1EC6-458C-BBD3-AF5AE0126D72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6EFFE9-2DF3-4A31-A58F-E8ABF0541401}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="18" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="390">
   <si>
     <t>00_Basedonnees'!A1</t>
   </si>
@@ -739,9 +739,6 @@
     <t>NCE</t>
   </si>
   <si>
-    <t>SELECT  Desordre.* , Objet.*, COUNT(nca.pk_observation) as ncacount, COUNT(ncb.pk_observation) as ncbcount , COUNT(ncc.pk_observation) as ncccount  FROM Desordre INNER JOIN Objet ON Desordre.lpk_objet = Objet.pk_objet LEFT JOIN Observation as nca ON nca.lid_desordre = Desordre.id_desordre AND nca.typeobservation = 'NCA' LEFT JOIN Observation as ncb ON ncb.lid_desordre = Desordre.id_desordre AND ncb.typeobservation = 'NCB'  LEFT JOIN Observation as ncc ON ncc.lid_desordre = Desordre.id_desordre AND ncc.typeobservation = 'NCC' LEFT JOIN Observation as ncd ON ncd.lid_desordre = Desordre.id_desordre AND ncd.typeobservation = 'NCD'  LEFT JOIN Observation as nce ON nce.lid_desordre = Desordre.id_desordre AND nce.typeobservation = 'NCE' GROUP BY Desordre.pk_desordre</t>
-  </si>
-  <si>
     <t>PV mise à disposition</t>
   </si>
   <si>
@@ -1196,6 +1193,21 @@
   </si>
   <si>
     <t>item_obs_40</t>
+  </si>
+  <si>
+    <t># SELECT  Desordre.* , Objet.*, COUNT(nca.pk_observation) as ncacount, COUNT(ncb.pk_observation) as ncbcount , COUNT(ncc.pk_observation) as ncccount  FROM Desordre INNER JOIN Objet ON Desordre.lpk_objet = Objet.pk_objet LEFT JOIN Observation as nca ON nca.lid_desordre = Desordre.id_desordre AND nca.typeobservation = 'NCA' LEFT JOIN Observation as ncb ON ncb.lid_desordre = Desordre.id_desordre AND ncb.typeobservation = 'NCB'  LEFT JOIN Observation as ncc ON ncc.lid_desordre = Desordre.id_desordre AND ncc.typeobservation = 'NCC' LEFT JOIN Observation as ncd ON ncd.lid_desordre = Desordre.id_desordre AND ncd.typeobservation = 'NCD'  LEFT JOIN Observation as nce ON nce.lid_desordre = Desordre.id_desordre AND nce.typeobservation = 'NCE' GROUP BY Desordre.pk_desordre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT  Desordre.* , Objet.*, COUNT(nca.pk_observation) as ncacount, COUNT(ncb.pk_observation) as ncbcount , COUNT(ncc.pk_observation) as ncccount  ,COUNT(SousObservation.pk_observation) as ncassfichenonconf
+FROM Desordre INNER JOIN Objet ON Desordre.lpk_objet = Objet.pk_objet 
+LEFT JOIN Observation as nca ON nca.lid_desordre = Desordre.id_desordre AND nca.typeobservation = 'NCA' 
+LEFT JOIN Observation as ncb ON ncb.lid_desordre = Desordre.id_desordre AND ncb.typeobservation = 'NCB'  
+LEFT JOIN Observation as ncc ON ncc.lid_desordre = Desordre.id_desordre AND ncc.typeobservation = 'NCC' 
+LEFT JOIN Observation as ncd ON ncd.lid_desordre = Desordre.id_desordre AND ncd.typeobservation = 'NCD'  
+LEFT JOIN Observation as nce ON nce.lid_desordre = Desordre.id_desordre AND nce.typeobservation = 'NCE' 
+LEFT JOIN Observation as SousObservation ON SousObservation.lid_observation = nca.id_observation 
+AND (SousObservation.item_type_1 = 0 OR SousObservation.item_type_2 = 0 OR SousObservation.item_type_3 = 0 OR SousObservation.item_type_4 = 0 OR SousObservation.item_type_5 = 0 OR SousObservation.item_type_6 = 0 OR SousObservation.item_type_7 = 0 OR SousObservation.item_type_8 = 0 OR SousObservation.item_type_9 = 0 OR SousObservation.item_type_10 = 0 OR SousObservation.item_type_11 = 0 OR SousObservation.item_type_12 = 0 OR SousObservation.item_type_13 = 0 OR SousObservation.item_type_14 = 0 OR SousObservation.item_type_15 = 0 OR SousObservation.item_type_16 = 0 OR SousObservation.item_type_17 = 0 OR SousObservation.item_type_18 = 0 OR SousObservation.item_type_19 = 0 OR SousObservation.item_type_20 = 0 OR SousObservation.item_type_21 = 0 OR SousObservation.item_type_22 = 0 OR SousObservation.item_type_23 = 0 OR SousObservation.item_type_24 = 0 OR SousObservation.item_type_25 = 0 OR SousObservation.item_type_26 = 0 OR SousObservation.item_type_27 = 0 OR SousObservation.item_type_28 = 0 OR SousObservation.item_type_29 = 0 OR SousObservation.item_type_30 = 0 OR SousObservation.item_type_31 = 0 OR SousObservation.item_type_32 = 0 OR SousObservation.item_type_33 = 0 OR SousObservation.item_type_34 = 0 OR SousObservation.item_type_35 = 0 OR SousObservation.item_type_36 = 0 OR SousObservation.item_type_37 = 0 OR SousObservation.item_type_38 = 0 OR SousObservation.item_type_39 = 0 OR SousObservation.item_type_40 = 0)
+GROUP BY Desordre.pk_desordre </t>
   </si>
 </sst>
 </file>
@@ -2267,10 +2279,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,140 +2297,138 @@
     <col min="11" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>222</v>
       </c>
-      <c r="B1" t="s">
-        <v>236</v>
+      <c r="B1" s="2" t="s">
+        <v>389</v>
       </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>388</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="F2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" t="s">
-        <v>249</v>
-      </c>
     </row>
     <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" t="s">
-        <v>100</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="F3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K3" t="s">
-        <v>103</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" t="s">
+        <v>102</v>
+      </c>
+      <c r="K4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>110</v>
       </c>
-      <c r="B6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I9" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="J9" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="J8" s="19" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F9" s="17" t="s">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
         <v>118</v>
@@ -2426,103 +2436,103 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>256</v>
-      </c>
-    </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="20" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="B20" t="s">
-        <v>118</v>
-      </c>
-      <c r="F20" s="11" t="s">
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F21" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F22" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G24" s="10" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="B24" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>257</v>
+      <c r="B26" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="B29" t="s">
-        <v>118</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B30" t="s">
         <v>118</v>
@@ -2530,15 +2540,15 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B32" t="s">
         <v>114</v>
@@ -2546,14 +2556,19 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="B33" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
@@ -2563,6 +2578,9 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2574,8 +2592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="D190" sqref="D190"/>
+    <sheetView topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="C184" sqref="C184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2820,7 +2838,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>108</v>
@@ -2879,10 +2897,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F34" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="G34" s="17" t="s">
         <v>237</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2891,14 +2909,14 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
@@ -3036,19 +3054,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B53"/>
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B55" t="s">
         <v>118</v>
@@ -3056,7 +3074,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B56" t="s">
         <v>118</v>
@@ -3064,12 +3082,12 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B58" t="s">
         <v>108</v>
@@ -3100,7 +3118,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B61" t="s">
         <v>118</v>
@@ -3112,12 +3130,12 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B64" t="s">
         <v>108</v>
@@ -3125,7 +3143,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B65" t="s">
         <v>108</v>
@@ -3133,7 +3151,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B66" t="s">
         <v>108</v>
@@ -3145,12 +3163,12 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B69" t="s">
         <v>108</v>
@@ -3158,7 +3176,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B70" t="s">
         <v>108</v>
@@ -3166,7 +3184,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B71" t="s">
         <v>108</v>
@@ -3174,7 +3192,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B72" t="s">
         <v>108</v>
@@ -3182,7 +3200,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B73" t="s">
         <v>108</v>
@@ -3190,7 +3208,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B74" t="s">
         <v>108</v>
@@ -3198,7 +3216,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B75" t="s">
         <v>108</v>
@@ -3206,7 +3224,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B76" t="s">
         <v>108</v>
@@ -3214,7 +3232,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B77" t="s">
         <v>108</v>
@@ -3222,7 +3240,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B78" t="s">
         <v>108</v>
@@ -3230,7 +3248,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B79" t="s">
         <v>108</v>
@@ -3238,7 +3256,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B80" t="s">
         <v>108</v>
@@ -3246,7 +3264,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B81" t="s">
         <v>108</v>
@@ -3254,7 +3272,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B82" t="s">
         <v>108</v>
@@ -3262,7 +3280,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B83" t="s">
         <v>108</v>
@@ -3270,12 +3288,12 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B86" s="20" t="s">
         <v>108</v>
@@ -3306,7 +3324,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B89" s="20" t="s">
         <v>108</v>
@@ -3335,7 +3353,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B92" s="20" t="s">
         <v>108</v>
@@ -3364,7 +3382,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B95" s="20" t="s">
         <v>108</v>
@@ -3393,7 +3411,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B98" s="20" t="s">
         <v>108</v>
@@ -3422,7 +3440,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B101" s="20" t="s">
         <v>108</v>
@@ -3451,7 +3469,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B104" s="20" t="s">
         <v>108</v>
@@ -3480,7 +3498,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B107" s="20" t="s">
         <v>108</v>
@@ -3509,7 +3527,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B110" s="20" t="s">
         <v>108</v>
@@ -3538,7 +3556,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B113" s="20" t="s">
         <v>108</v>
@@ -3567,7 +3585,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B116" s="20" t="s">
         <v>108</v>
@@ -3596,7 +3614,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B119" s="20" t="s">
         <v>108</v>
@@ -3625,7 +3643,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B122" s="20" t="s">
         <v>108</v>
@@ -3654,7 +3672,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B125" s="20" t="s">
         <v>108</v>
@@ -3683,7 +3701,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B128" s="20" t="s">
         <v>108</v>
@@ -3711,7 +3729,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B131" t="s">
         <v>118</v>
@@ -3833,7 +3851,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -4034,7 +4052,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>130</v>
@@ -4042,7 +4060,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B176" t="s">
         <v>118</v>
@@ -4050,7 +4068,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B178" t="s">
         <v>108</v>
@@ -4058,7 +4076,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B179" t="s">
         <v>108</v>
@@ -4066,7 +4084,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B180" t="s">
         <v>108</v>
@@ -4074,7 +4092,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>130</v>
@@ -4082,7 +4100,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B183" t="s">
         <v>108</v>
@@ -4090,7 +4108,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B184" t="s">
         <v>108</v>
@@ -4098,7 +4116,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B185" t="s">
         <v>108</v>
@@ -4106,7 +4124,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>130</v>
@@ -4114,12 +4132,12 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B189" t="s">
         <v>118</v>
@@ -4127,7 +4145,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B191" s="20" t="s">
         <v>108</v>
@@ -4135,7 +4153,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B192" t="s">
         <v>118</v>
@@ -4143,7 +4161,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B193" s="20" t="s">
         <v>108</v>
@@ -4151,7 +4169,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B194" t="s">
         <v>118</v>
@@ -4159,7 +4177,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B195" s="20" t="s">
         <v>108</v>
@@ -4167,7 +4185,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B196" t="s">
         <v>118</v>
@@ -4175,7 +4193,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B197" s="20" t="s">
         <v>108</v>
@@ -4183,7 +4201,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B198" t="s">
         <v>118</v>
@@ -4191,7 +4209,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B199" s="20" t="s">
         <v>108</v>
@@ -4199,7 +4217,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B200" t="s">
         <v>118</v>
@@ -4207,7 +4225,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B201" s="20" t="s">
         <v>108</v>
@@ -4215,7 +4233,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B202" t="s">
         <v>118</v>
@@ -4223,7 +4241,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B203" s="20" t="s">
         <v>108</v>
@@ -4231,7 +4249,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B204" t="s">
         <v>118</v>
@@ -4239,7 +4257,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B205" s="20" t="s">
         <v>108</v>
@@ -4247,7 +4265,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B206" t="s">
         <v>118</v>
@@ -4255,7 +4273,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B207" s="20" t="s">
         <v>108</v>
@@ -4263,7 +4281,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B208" t="s">
         <v>118</v>
@@ -4271,7 +4289,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B209" s="20" t="s">
         <v>108</v>
@@ -4279,7 +4297,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B210" t="s">
         <v>118</v>
@@ -4287,7 +4305,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B211" s="20" t="s">
         <v>108</v>
@@ -4295,7 +4313,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B212" t="s">
         <v>118</v>
@@ -4303,7 +4321,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B213" s="20" t="s">
         <v>108</v>
@@ -4311,7 +4329,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B214" t="s">
         <v>118</v>
@@ -4319,7 +4337,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B215" s="20" t="s">
         <v>108</v>
@@ -4327,7 +4345,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B216" t="s">
         <v>118</v>
@@ -4335,7 +4353,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B217" s="20" t="s">
         <v>108</v>
@@ -4343,7 +4361,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B218" t="s">
         <v>118</v>
@@ -4351,7 +4369,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B219" s="20" t="s">
         <v>108</v>
@@ -4359,7 +4377,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B220" t="s">
         <v>118</v>
@@ -4367,7 +4385,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B221" s="20" t="s">
         <v>108</v>
@@ -4375,7 +4393,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B222" t="s">
         <v>118</v>
@@ -4383,7 +4401,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B223" s="20" t="s">
         <v>108</v>
@@ -4391,7 +4409,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B224" t="s">
         <v>118</v>
@@ -4399,7 +4417,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B225" s="20" t="s">
         <v>108</v>
@@ -4407,7 +4425,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B226" t="s">
         <v>118</v>
@@ -4415,7 +4433,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B227" s="20" t="s">
         <v>108</v>
@@ -4423,7 +4441,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B228" t="s">
         <v>118</v>
@@ -4431,7 +4449,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B229" s="20" t="s">
         <v>108</v>
@@ -4439,7 +4457,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B230" t="s">
         <v>118</v>
@@ -4447,7 +4465,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B231" s="20" t="s">
         <v>108</v>
@@ -4455,7 +4473,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B232" t="s">
         <v>118</v>
@@ -4463,7 +4481,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B233" s="20" t="s">
         <v>108</v>
@@ -4471,7 +4489,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B234" t="s">
         <v>118</v>
@@ -4479,7 +4497,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B235" s="20" t="s">
         <v>108</v>
@@ -4487,7 +4505,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B236" t="s">
         <v>118</v>
@@ -4495,7 +4513,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B237" s="20" t="s">
         <v>108</v>
@@ -4503,7 +4521,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B238" t="s">
         <v>118</v>
@@ -4511,7 +4529,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B239" s="20" t="s">
         <v>108</v>
@@ -4519,7 +4537,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B240" t="s">
         <v>118</v>
@@ -4527,7 +4545,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B241" s="20" t="s">
         <v>108</v>
@@ -4535,7 +4553,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B242" t="s">
         <v>118</v>
@@ -4543,7 +4561,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B243" s="20" t="s">
         <v>108</v>
@@ -4551,7 +4569,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B244" t="s">
         <v>118</v>
@@ -4559,7 +4577,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B245" s="20" t="s">
         <v>108</v>
@@ -4567,7 +4585,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B246" t="s">
         <v>118</v>
@@ -4575,7 +4593,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="20" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B247" s="20" t="s">
         <v>108</v>
@@ -4583,7 +4601,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B248" t="s">
         <v>118</v>
@@ -4591,7 +4609,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B249" s="20" t="s">
         <v>108</v>
@@ -4599,7 +4617,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B250" t="s">
         <v>118</v>
@@ -4607,7 +4625,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="20" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B251" s="20" t="s">
         <v>108</v>
@@ -4615,7 +4633,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B252" t="s">
         <v>118</v>
@@ -4623,7 +4641,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="20" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B253" s="20" t="s">
         <v>108</v>
@@ -4631,7 +4649,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="20" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B254" t="s">
         <v>118</v>
@@ -4639,7 +4657,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="20" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B255" s="20" t="s">
         <v>108</v>
@@ -4647,7 +4665,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="20" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B256" t="s">
         <v>118</v>
@@ -4655,7 +4673,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B257" s="20" t="s">
         <v>108</v>
@@ -4663,7 +4681,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B258" t="s">
         <v>118</v>
@@ -4671,7 +4689,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B259" s="20" t="s">
         <v>108</v>
@@ -4679,7 +4697,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="20" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B260" t="s">
         <v>118</v>
@@ -4687,7 +4705,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B261" s="20" t="s">
         <v>108</v>
@@ -4695,7 +4713,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="20" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B262" t="s">
         <v>118</v>
@@ -4703,7 +4721,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="20" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B263" s="20" t="s">
         <v>108</v>
@@ -4711,7 +4729,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B264" t="s">
         <v>118</v>
@@ -4719,7 +4737,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B265" s="20" t="s">
         <v>108</v>
@@ -4727,7 +4745,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B266" t="s">
         <v>118</v>
@@ -4735,7 +4753,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="20" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B267" s="20" t="s">
         <v>108</v>
@@ -4743,7 +4761,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="20" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B268" t="s">
         <v>118</v>
@@ -4751,7 +4769,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="20" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B269" s="20" t="s">
         <v>108</v>
@@ -4759,7 +4777,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B270" t="s">
         <v>118</v>

</xml_diff>